<commit_message>
asta reportes FINAL CLASE LUNES 28
</commit_message>
<xml_diff>
--- a/reportes/hello_world.xlsx
+++ b/reportes/hello_world.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
   <si>
-    <t>Hello World !</t>
+    <t>LISTA DE PRECIOS !</t>
   </si>
 </sst>
 </file>
@@ -357,7 +357,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -365,8 +365,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
+    <row r="3" spans="1:3">
+      <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>